<commit_message>
Fix file paths for Windows wit row strings
</commit_message>
<xml_diff>
--- a/EcoDynBat_tests.xlsx
+++ b/EcoDynBat_tests.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Parameter" sheetId="1" state="visible" r:id="rId2"/>
@@ -86,13 +86,13 @@
     <t xml:space="preserve">generation directory</t>
   </si>
   <si>
-    <t xml:space="preserve">../Generation_Data/</t>
+    <t xml:space="preserve">../../Calculs_EcoDynBat/Generation_Data/</t>
   </si>
   <si>
     <t xml:space="preserve">exchange directory</t>
   </si>
   <si>
-    <t xml:space="preserve">../Importation_Data/</t>
+    <t xml:space="preserve">../../Calculs_EcoDynBat/Importation_Data/</t>
   </si>
   <si>
     <t xml:space="preserve">saving directory</t>
@@ -101,7 +101,7 @@
     <t xml:space="preserve">mapping file</t>
   </si>
   <si>
-    <t xml:space="preserve">../Mappings/Mapping_case_residue_mean.xlsx</t>
+    <t xml:space="preserve">../../Calculs_EcoDynBat/Mappings/Mapping_case_residue_mean.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">neighboring file</t>
@@ -228,14 +228,15 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -397,14 +398,15 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.5714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="46.030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>